<commit_message>
updated theoretical HR diagram
</commit_message>
<xml_diff>
--- a/Inst/Data/Extdata/mcdonaldstars.xlsx
+++ b/Inst/Data/Extdata/mcdonaldstars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonygojanovic/Data/R Projects/Hertzsprung-Russell/Inst/Data/Extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonygojanovic/Data/R Projects/Hertzsprung-Russell/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA60931D-B791-314D-8D35-B2117A6A8C09}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F979E1AE-F83D-5C4F-AA0B-8DAFFBC3D47E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="540" windowWidth="18460" windowHeight="14340" xr2:uid="{F7E7B911-20A1-644E-93D1-2BA2D9C210D7}"/>
+    <workbookView xWindow="15600" yWindow="460" windowWidth="10000" windowHeight="14560" xr2:uid="{F7E7B911-20A1-644E-93D1-2BA2D9C210D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="230">
   <si>
     <t>Sun</t>
   </si>
@@ -2711,13 +2711,167 @@
   </si>
   <si>
     <t>light_years</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>US 708</t>
+  </si>
+  <si>
+    <t>LP 40-365</t>
+  </si>
+  <si>
+    <t>D6-1</t>
+  </si>
+  <si>
+    <t>Apus</t>
+  </si>
+  <si>
+    <t>Hypervelocity star at 1060 km per sec</t>
+  </si>
+  <si>
+    <t>Hypervelocity star at 2300 km per sec</t>
+  </si>
+  <si>
+    <t>Hypervelocity star at 850 km per sec</t>
+  </si>
+  <si>
+    <t>D6-2</t>
+  </si>
+  <si>
+    <t>Hypervelocity star at 1300 km per sec</t>
+  </si>
+  <si>
+    <t>D6-3</t>
+  </si>
+  <si>
+    <t>Draco</t>
+  </si>
+  <si>
+    <t>Hypervelocity star at 2400 km per sec</t>
+  </si>
+  <si>
+    <t>Pegasus</t>
+  </si>
+  <si>
+    <r>
+      <t>09</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> 33</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> 20.865</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <t>+44° 17′ 05.52″</t>
+  </si>
+  <si>
+    <r>
+      <t>14</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> 06</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> 35.45</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <t>+74° 18′ 58.0″</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2735,6 +2889,19 @@
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2759,7 +2926,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2768,6 +2935,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3082,1649 +3258,1958 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3715CC-A559-B540-81D3-3BB48DFBC09B}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="8.5" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>205</v>
       </c>
       <c r="B1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" t="s">
         <v>206</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>207</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>208</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>209</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>210</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="1">
-        <v>5.2</v>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D2" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="E2" s="2">
-        <v>4000</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>54</v>
+        <v>12.3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>14.7</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2500</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" t="s">
-        <v>58</v>
+        <v>91</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="I2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J2">
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="1">
-        <v>6.05</v>
-      </c>
-      <c r="D3" s="1">
-        <v>8.33</v>
-      </c>
-      <c r="E3" s="2">
-        <v>4077</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J3">
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="J2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" s="5">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E3" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="F3" s="6">
+        <v>8000</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="K3" s="4">
+        <v>6900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1">
-        <v>9.5</v>
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D4" s="1">
-        <v>13.2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2600</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>60</v>
+        <v>12.3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>14.9</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2500</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" t="s">
-        <v>59</v>
+        <v>99</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="I4" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="J4" t="s">
+        <v>102</v>
+      </c>
+      <c r="K4">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1">
-        <v>7.5</v>
+      <c r="B5" s="8">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D5" s="1">
-        <v>10.5</v>
-      </c>
-      <c r="E5" s="2">
-        <v>2700</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>94</v>
+        <v>12.3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>15.9</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2200</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H5" t="s">
-        <v>64</v>
+        <v>99</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="I5" t="s">
-        <v>96</v>
-      </c>
-      <c r="J5">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="J5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K5">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1">
-        <v>8.1</v>
+        <v>46</v>
+      </c>
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="D6" s="1">
-        <v>10.3</v>
-      </c>
-      <c r="E6" s="2">
-        <v>2950</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.8</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F6" s="2">
+        <v>7700</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I6" t="s">
+        <v>136</v>
+      </c>
+      <c r="J6" t="s">
+        <v>137</v>
+      </c>
+      <c r="K6">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1">
-        <v>11.1</v>
+        <v>46</v>
+      </c>
+      <c r="B7" s="8">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D7" s="1">
-        <v>13.2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-0.7</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I7" t="s">
+        <v>155</v>
+      </c>
+      <c r="J7" t="s">
+        <v>156</v>
+      </c>
+      <c r="K7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="1">
-        <v>8.9</v>
+        <v>46</v>
+      </c>
+      <c r="B8" s="8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="D8" s="1">
-        <v>11.1</v>
-      </c>
-      <c r="E8" s="2">
-        <v>2650</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3200</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I8" t="s">
+        <v>155</v>
+      </c>
+      <c r="J8" t="s">
+        <v>156</v>
+      </c>
+      <c r="K8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="1">
-        <v>9.6999999999999993</v>
+        <v>46</v>
+      </c>
+      <c r="B9" s="8">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D9" s="1">
-        <v>11.9</v>
-      </c>
-      <c r="E9" s="2">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>-0.1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-0.3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3900</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I9" t="s">
+        <v>144</v>
+      </c>
+      <c r="J9" t="s">
+        <v>145</v>
+      </c>
+      <c r="K9">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1">
-        <v>3.7</v>
+      <c r="B10" s="8">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D10" s="1">
-        <v>6.1</v>
-      </c>
-      <c r="E10" s="2">
-        <v>4500</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>71</v>
+        <v>-1.4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="F10" s="2">
+        <v>9500</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" t="s">
-        <v>73</v>
+        <v>103</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="I10" t="s">
-        <v>189</v>
-      </c>
-      <c r="J10">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="J10" t="s">
+        <v>188</v>
+      </c>
+      <c r="K10">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1">
-        <v>12.6</v>
+      <c r="B11" s="8">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D11" s="1">
-        <v>15.4</v>
-      </c>
-      <c r="E11" s="2">
-        <v>2500</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>97</v>
+        <v>8.4</v>
+      </c>
+      <c r="E11" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>28000</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H11" t="s">
-        <v>68</v>
+        <v>105</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="I11" t="s">
-        <v>90</v>
-      </c>
-      <c r="J11">
-        <v>8.6999999999999993</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="J11" t="s">
+        <v>108</v>
+      </c>
+      <c r="K11">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1">
-        <v>13</v>
+      <c r="B12" s="8">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D12" s="1">
-        <v>15.8</v>
-      </c>
-      <c r="E12" s="2">
-        <v>2400</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>97</v>
+        <v>0.4</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="F12" s="2">
+        <v>6500</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H12" t="s">
-        <v>68</v>
+        <v>74</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="I12" t="s">
-        <v>190</v>
-      </c>
-      <c r="J12">
-        <v>8.6999999999999993</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="J12" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="1">
-        <v>12.3</v>
+      <c r="B13" s="8">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="D13" s="1">
-        <v>14.9</v>
-      </c>
-      <c r="E13" s="2">
-        <v>2500</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>99</v>
+        <v>10.7</v>
+      </c>
+      <c r="E13" s="1">
+        <v>13</v>
+      </c>
+      <c r="F13" s="2">
+        <v>7000</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H13" t="s">
-        <v>101</v>
+        <v>74</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="I13" t="s">
-        <v>102</v>
-      </c>
-      <c r="J13">
-        <v>11.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="J13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="1">
-        <v>12.3</v>
+        <v>46</v>
+      </c>
+      <c r="B14" s="8">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D14" s="1">
-        <v>15.9</v>
-      </c>
-      <c r="E14" s="2">
-        <v>2200</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>99</v>
+        <v>-0.6</v>
+      </c>
+      <c r="E14" s="1">
+        <v>-3.1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>6400</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H14" t="s">
-        <v>101</v>
+        <v>149</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="I14" t="s">
-        <v>102</v>
-      </c>
-      <c r="J14">
-        <v>11.1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+      <c r="J14" t="s">
+        <v>152</v>
+      </c>
+      <c r="K14">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0.4</v>
+        <v>47</v>
+      </c>
+      <c r="B15" s="8">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="D15" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="E15" s="2">
-        <v>6500</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>74</v>
+        <v>4.5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>-9.5</v>
+      </c>
+      <c r="F15" s="2">
+        <v>5200</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" t="s">
-        <v>76</v>
+        <v>66</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="I15" t="s">
-        <v>81</v>
-      </c>
-      <c r="J15">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="J15" t="s">
+        <v>186</v>
+      </c>
+      <c r="K15">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="1">
-        <v>10.7</v>
+      <c r="B16" s="8">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D16" s="1">
-        <v>13</v>
-      </c>
-      <c r="E16" s="2">
-        <v>7000</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>74</v>
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5800</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H16" t="s">
-        <v>76</v>
+        <v>113</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="I16" t="s">
-        <v>80</v>
-      </c>
-      <c r="J16">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="J16" t="s">
+        <v>118</v>
+      </c>
+      <c r="K16">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="1">
-        <v>11.1</v>
+      <c r="B17" s="8">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="D17" s="1">
-        <v>13.5</v>
-      </c>
-      <c r="E17" s="2">
-        <v>2600</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>77</v>
+        <v>1.4</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="F17" s="2">
+        <v>4000</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H17" t="s">
-        <v>79</v>
+        <v>115</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="I17" t="s">
-        <v>90</v>
-      </c>
-      <c r="J17">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="J17" t="s">
+        <v>119</v>
+      </c>
+      <c r="K17">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="8">
         <v>17</v>
       </c>
-      <c r="C18" s="1">
-        <v>10.4</v>
+      <c r="C18" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="D18" s="1">
-        <v>13.3</v>
-      </c>
-      <c r="E18" s="2">
-        <v>2650</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>87</v>
+        <v>11</v>
+      </c>
+      <c r="E18" s="1">
+        <v>15.8</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2600</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="H18" t="s">
-        <v>89</v>
+        <v>115</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="I18" t="s">
-        <v>90</v>
-      </c>
-      <c r="J18">
-        <v>9.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="J18" t="s">
+        <v>110</v>
+      </c>
+      <c r="K18">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="8">
         <v>18</v>
       </c>
-      <c r="C19" s="1">
-        <v>12.3</v>
+      <c r="C19" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D19" s="1">
-        <v>14.7</v>
-      </c>
-      <c r="E19" s="2">
-        <v>2500</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>91</v>
+        <v>0.6</v>
+      </c>
+      <c r="E19" s="1">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="F19" s="2">
+        <v>20000</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="H19" t="s">
-        <v>93</v>
+        <v>194</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>195</v>
       </c>
       <c r="I19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J19">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="J19" t="s">
+        <v>196</v>
+      </c>
+      <c r="K19">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="1">
-        <v>-1.4</v>
+      <c r="B20" s="8">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D20" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="E20" s="2">
-        <v>9500</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>103</v>
+        <v>12.6</v>
+      </c>
+      <c r="E20" s="1">
+        <v>15.4</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2500</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="H20" t="s">
-        <v>107</v>
+        <v>97</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="I20" t="s">
-        <v>188</v>
-      </c>
-      <c r="J20">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="J20" t="s">
+        <v>90</v>
+      </c>
+      <c r="K20">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="1">
-        <v>8.4</v>
+      <c r="B21" s="8">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D21" s="1">
-        <v>8.4</v>
-      </c>
-      <c r="E21" s="2">
-        <v>28000</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>105</v>
+        <v>13</v>
+      </c>
+      <c r="E21" s="1">
+        <v>15.8</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2400</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="H21" t="s">
-        <v>107</v>
+        <v>97</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="I21" t="s">
-        <v>108</v>
-      </c>
-      <c r="J21">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="J21" t="s">
+        <v>190</v>
+      </c>
+      <c r="K21">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="1">
-        <v>13.5</v>
+        <v>47</v>
+      </c>
+      <c r="B22" s="8">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="D22" s="1">
-        <v>16.8</v>
-      </c>
-      <c r="E22" s="2">
-        <v>2400</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>111</v>
+        <v>14.1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>12.3</v>
+      </c>
+      <c r="F22" s="2">
+        <v>10300</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="H22" t="s">
-        <v>109</v>
+        <v>69</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="I22" t="s">
-        <v>90</v>
-      </c>
-      <c r="J22">
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="J22" t="s">
+        <v>187</v>
+      </c>
+      <c r="K22">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0</v>
+        <v>46</v>
+      </c>
+      <c r="B23" s="8">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="D23" s="1">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E23" s="2">
-        <v>5800</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>113</v>
+        <v>0.9</v>
+      </c>
+      <c r="E23" s="1">
+        <v>-4</v>
+      </c>
+      <c r="F23" s="2">
+        <v>19500</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H23" t="s">
-        <v>117</v>
+        <v>198</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="I23" t="s">
-        <v>118</v>
-      </c>
-      <c r="J23">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+      <c r="J23" t="s">
+        <v>200</v>
+      </c>
+      <c r="K23">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1.4</v>
+        <v>46</v>
+      </c>
+      <c r="B24" s="8">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="D24" s="1">
-        <v>5.8</v>
-      </c>
-      <c r="E24" s="2">
-        <v>4000</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>115</v>
+        <v>0.9</v>
+      </c>
+      <c r="E24" s="1">
+        <v>-3.5</v>
+      </c>
+      <c r="F24" s="2">
+        <v>16500</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H24" t="s">
-        <v>117</v>
+        <v>198</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="I24" t="s">
-        <v>119</v>
-      </c>
-      <c r="J24">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+      <c r="J24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K24">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C25" s="1">
-        <v>11</v>
+        <v>46</v>
+      </c>
+      <c r="B25" s="8">
+        <v>24</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D25" s="1">
-        <v>15.8</v>
-      </c>
-      <c r="E25" s="2">
-        <v>2600</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>115</v>
+        <v>1.3</v>
+      </c>
+      <c r="E25" s="1">
+        <v>-4</v>
+      </c>
+      <c r="F25" s="2">
+        <v>29000</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H25" t="s">
-        <v>117</v>
+        <v>201</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="I25" t="s">
-        <v>110</v>
-      </c>
-      <c r="J25">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+      <c r="J25" t="s">
+        <v>81</v>
+      </c>
+      <c r="K25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="1">
-        <v>4.7</v>
+      <c r="B26" s="8">
+        <v>25</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D26" s="1">
-        <v>7</v>
-      </c>
-      <c r="E26" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="F26" s="2">
         <v>4000</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="G26" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H26" t="s">
-        <v>122</v>
+        <v>54</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="I26" t="s">
-        <v>123</v>
-      </c>
-      <c r="J26">
-        <v>11.8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="1">
-        <v>0.5</v>
+        <v>58</v>
+      </c>
+      <c r="J26" t="s">
+        <v>85</v>
+      </c>
+      <c r="K26">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="8">
+        <v>26</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="D27" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E27" s="2">
-        <v>13500</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>124</v>
+        <v>6.05</v>
+      </c>
+      <c r="E27" s="1">
+        <v>8.33</v>
+      </c>
+      <c r="F27" s="2">
+        <v>4077</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H27" t="s">
-        <v>73</v>
+        <v>83</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="I27" t="s">
-        <v>126</v>
-      </c>
-      <c r="J27">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="J27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K27">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="1">
-        <v>0.9</v>
+      <c r="B28" s="8">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D28" s="1">
-        <v>-0.2</v>
-      </c>
-      <c r="E28" s="2">
-        <v>3500</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>127</v>
+        <v>1.3</v>
+      </c>
+      <c r="E28" s="1">
+        <v>-7.5</v>
+      </c>
+      <c r="F28" s="2">
+        <v>9080</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="H28" t="s">
-        <v>129</v>
+        <v>157</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="I28" t="s">
-        <v>191</v>
-      </c>
-      <c r="J28">
-        <v>65.3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D29" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E29" s="2">
-        <v>7700</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="H29" t="s">
-        <v>136</v>
-      </c>
-      <c r="I29" t="s">
-        <v>137</v>
-      </c>
-      <c r="J29">
-        <v>16.7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="J28" t="s">
+        <v>159</v>
+      </c>
+      <c r="K28">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="8">
+        <v>28</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D29" s="5">
+        <v>18.3</v>
+      </c>
+      <c r="E29" s="5">
+        <v>6.3</v>
+      </c>
+      <c r="F29" s="6">
+        <v>8000</v>
+      </c>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="K29" s="4">
+        <v>7600</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="B30" s="8">
+        <v>29</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D30" s="1">
-        <v>-4.5</v>
-      </c>
-      <c r="E30" s="2">
-        <v>2700</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>138</v>
+        <v>3.7</v>
+      </c>
+      <c r="E30" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="F30" s="2">
+        <v>4500</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="H30" t="s">
-        <v>140</v>
+        <v>71</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="I30" t="s">
-        <v>141</v>
-      </c>
-      <c r="J30">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="J30" t="s">
+        <v>189</v>
+      </c>
+      <c r="K30">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="1">
-        <v>-0.1</v>
+      <c r="B31" s="8">
+        <v>30</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D31" s="1">
-        <v>-0.3</v>
-      </c>
-      <c r="E31" s="2">
-        <v>3900</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>142</v>
+        <v>0.5</v>
+      </c>
+      <c r="E31" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F31" s="2">
+        <v>13500</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="H31" t="s">
-        <v>144</v>
+        <v>124</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="I31" t="s">
-        <v>145</v>
-      </c>
-      <c r="J31">
-        <v>36.700000000000003</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="J31" t="s">
+        <v>126</v>
+      </c>
+      <c r="K31">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="1">
-        <v>0.5</v>
+      <c r="B32" s="8">
+        <v>31</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D32" s="1">
-        <v>-5.5</v>
-      </c>
-      <c r="E32" s="2">
-        <v>2700</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>146</v>
+        <v>1.2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F32" s="2">
+        <v>4100</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="H32" t="s">
-        <v>148</v>
+        <v>164</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="I32" t="s">
-        <v>141</v>
-      </c>
-      <c r="J32">
-        <v>642.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+      <c r="J32" t="s">
+        <v>167</v>
+      </c>
+      <c r="K32">
+        <v>33.799999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="8">
+        <v>32</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="E33" s="1">
+        <v>7</v>
+      </c>
+      <c r="F33" s="2">
+        <v>4000</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I33" t="s">
+        <v>122</v>
+      </c>
+      <c r="J33" t="s">
+        <v>123</v>
+      </c>
+      <c r="K33">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="8">
         <v>33</v>
       </c>
-      <c r="C33" s="1">
-        <v>-0.6</v>
-      </c>
-      <c r="D33" s="1">
-        <v>-3.1</v>
-      </c>
-      <c r="E33" s="2">
-        <v>6400</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="H33" t="s">
-        <v>151</v>
-      </c>
-      <c r="I33" t="s">
-        <v>152</v>
-      </c>
-      <c r="J33">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="1">
-        <v>0.1</v>
+      <c r="C34" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D34" s="1">
-        <v>-0.7</v>
-      </c>
-      <c r="E34" s="2">
-        <v>5000</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>153</v>
+        <v>13.5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>16.8</v>
+      </c>
+      <c r="F34" s="2">
+        <v>2400</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="H34" t="s">
-        <v>155</v>
+        <v>111</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="I34" t="s">
-        <v>156</v>
-      </c>
-      <c r="J34">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="J34" t="s">
+        <v>90</v>
+      </c>
+      <c r="K34">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="1">
-        <v>0.1</v>
+      <c r="B35" s="8">
+        <v>34</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="D35" s="1">
-        <v>9.5</v>
-      </c>
-      <c r="E35" s="2">
-        <v>3200</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>153</v>
+        <v>1.4</v>
+      </c>
+      <c r="E35" s="1">
+        <v>-0.6</v>
+      </c>
+      <c r="F35" s="2">
+        <v>13000</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="H35" t="s">
-        <v>155</v>
+        <v>168</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="I35" t="s">
-        <v>156</v>
-      </c>
-      <c r="J35">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="J35" t="s">
+        <v>170</v>
+      </c>
+      <c r="K35">
+        <v>79.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="1">
-        <v>1.3</v>
+      <c r="B36" s="8">
+        <v>35</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="D36" s="1">
-        <v>-7.5</v>
-      </c>
-      <c r="E36" s="2">
-        <v>9080</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>157</v>
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F36" s="2">
+        <v>9700</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H36" t="s">
-        <v>58</v>
+        <v>178</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="I36" t="s">
-        <v>159</v>
-      </c>
-      <c r="J36">
-        <v>2615</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="J36" t="s">
+        <v>192</v>
+      </c>
+      <c r="K36">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="1">
-        <v>1.2</v>
+        <v>31</v>
+      </c>
+      <c r="B37" s="8">
+        <v>36</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D37" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="E37" s="2">
-        <v>8720</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>160</v>
+        <v>9.5</v>
+      </c>
+      <c r="E37" s="1">
+        <v>13.2</v>
+      </c>
+      <c r="F37" s="2">
+        <v>2600</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H37" t="s">
-        <v>162</v>
+        <v>60</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="I37" t="s">
-        <v>163</v>
-      </c>
-      <c r="J37">
-        <v>25.1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="J37" t="s">
+        <v>86</v>
+      </c>
+      <c r="K37">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1.2</v>
+      <c r="B38" s="8">
+        <v>37</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="D38" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E38" s="2">
-        <v>4100</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>164</v>
+        <v>0.5</v>
+      </c>
+      <c r="E38" s="1">
+        <v>-5.5</v>
+      </c>
+      <c r="F38" s="2">
+        <v>2700</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="H38" t="s">
-        <v>166</v>
+        <v>146</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="I38" t="s">
-        <v>167</v>
-      </c>
-      <c r="J38">
-        <v>33.799999999999997</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="J38" t="s">
+        <v>141</v>
+      </c>
+      <c r="K38">
+        <v>642.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="1">
-        <v>1.4</v>
+      <c r="B39" s="8">
+        <v>38</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D39" s="1">
-        <v>-0.6</v>
-      </c>
-      <c r="E39" s="2">
-        <v>13000</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>168</v>
+        <v>0.2</v>
+      </c>
+      <c r="E39" s="1">
+        <v>-6.8</v>
+      </c>
+      <c r="F39" s="2">
+        <v>11000</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="H39" t="s">
-        <v>109</v>
+        <v>171</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="I39" t="s">
-        <v>170</v>
-      </c>
-      <c r="J39">
-        <v>79.3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D40" s="1">
-        <v>-6.8</v>
-      </c>
-      <c r="E40" s="2">
-        <v>11000</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H40" t="s">
         <v>148</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J39" t="s">
         <v>173</v>
       </c>
-      <c r="J40">
+      <c r="K39">
         <v>863</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="8">
+        <v>39</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D40" s="5">
+        <v>17</v>
+      </c>
+      <c r="E40" s="5">
+        <v>6.9</v>
+      </c>
+      <c r="F40" s="6">
+        <v>8000</v>
+      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="K40" s="4">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1</v>
+      <c r="B41" s="8">
+        <v>40</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D41" s="1">
-        <v>-3.6</v>
-      </c>
-      <c r="E41" s="2">
-        <v>19500</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>174</v>
+        <v>1.2</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="F41" s="2">
+        <v>8720</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="H41" t="s">
-        <v>79</v>
+        <v>160</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="I41" t="s">
-        <v>176</v>
-      </c>
-      <c r="J41">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+      <c r="J41" t="s">
+        <v>163</v>
+      </c>
+      <c r="K41">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="1">
-        <v>-26.8</v>
+        <v>31</v>
+      </c>
+      <c r="B42" s="8">
+        <v>41</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D42" s="1">
-        <v>4.8</v>
-      </c>
-      <c r="E42" s="2">
-        <v>5770</v>
+        <v>10.4</v>
+      </c>
+      <c r="E42" s="1">
+        <v>13.3</v>
+      </c>
+      <c r="F42" s="2">
+        <v>2650</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="I42" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="J42" t="s">
+        <v>90</v>
+      </c>
+      <c r="K42">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="1">
-        <v>0</v>
+      <c r="B43" s="8">
+        <v>42</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="D43" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E43" s="2">
-        <v>9700</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>178</v>
+        <v>1</v>
+      </c>
+      <c r="E43" s="1">
+        <v>-4.5</v>
+      </c>
+      <c r="F43" s="2">
+        <v>2700</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="H43" t="s">
-        <v>180</v>
+        <v>138</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="I43" t="s">
-        <v>192</v>
-      </c>
-      <c r="J43">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+      <c r="J43" t="s">
+        <v>141</v>
+      </c>
+      <c r="K43">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44" s="1">
+      <c r="B44" s="8">
+        <v>43</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="1">
         <v>0.9</v>
       </c>
-      <c r="D44" s="1">
-        <v>-4</v>
-      </c>
-      <c r="E44" s="2">
-        <v>19500</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>198</v>
+      <c r="E44" s="1">
+        <v>-0.2</v>
+      </c>
+      <c r="F44" s="2">
+        <v>3500</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="H44" t="s">
-        <v>197</v>
+        <v>127</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="I44" t="s">
-        <v>200</v>
-      </c>
-      <c r="J44">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="J44" t="s">
+        <v>191</v>
+      </c>
+      <c r="K44">
+        <v>65.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="8">
+        <v>44</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="E45" s="1">
+        <v>-0.2</v>
+      </c>
+      <c r="F45" s="2">
+        <v>9520</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="I45" t="s">
+        <v>132</v>
+      </c>
+      <c r="J45" t="s">
+        <v>203</v>
+      </c>
+      <c r="K45">
+        <v>82.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="8">
+        <v>45</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F46" s="2">
+        <v>9520</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="I46" t="s">
+        <v>132</v>
+      </c>
+      <c r="J46" t="s">
+        <v>181</v>
+      </c>
+      <c r="K46">
+        <v>79.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="8">
         <v>46</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="D45" s="1">
-        <v>-3.5</v>
-      </c>
-      <c r="E45" s="2">
-        <v>16500</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="H45" t="s">
-        <v>197</v>
-      </c>
-      <c r="I45" t="s">
-        <v>200</v>
-      </c>
-      <c r="J45">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="D46" s="1">
-        <v>-4.0999999999999996</v>
-      </c>
-      <c r="E46" s="2">
-        <v>20000</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="H46" t="s">
-        <v>117</v>
-      </c>
-      <c r="I46" t="s">
-        <v>196</v>
-      </c>
-      <c r="J46">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1.3</v>
+      <c r="C47" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D47" s="1">
-        <v>-4</v>
-      </c>
-      <c r="E47" s="2">
-        <v>29000</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>201</v>
+        <v>1.8</v>
+      </c>
+      <c r="E47" s="1">
+        <v>-1.3</v>
+      </c>
+      <c r="F47" s="2">
+        <v>4750</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="H47" t="s">
-        <v>197</v>
+        <v>130</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="I47" t="s">
-        <v>81</v>
-      </c>
-      <c r="J47">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+        <v>132</v>
+      </c>
+      <c r="J47" t="s">
+        <v>133</v>
+      </c>
+      <c r="K47">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="8">
         <v>47</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D48" s="5">
+        <v>18.7</v>
+      </c>
+      <c r="E48" s="5">
+        <v>4</v>
+      </c>
+      <c r="F48" s="6">
+        <v>47000</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="K48" s="4">
+        <v>28000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="8">
         <v>48</v>
       </c>
-      <c r="C48" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="D48" s="1">
-        <v>-0.2</v>
-      </c>
-      <c r="E48" s="2">
-        <v>9520</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H48" t="s">
-        <v>132</v>
-      </c>
-      <c r="I48" t="s">
-        <v>203</v>
-      </c>
-      <c r="J48">
-        <v>82.6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C49" s="1">
-        <v>2.2999999999999998</v>
+      <c r="C49" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D49" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="E49" s="2">
-        <v>9520</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>184</v>
+        <v>7.5</v>
+      </c>
+      <c r="E49" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="F49" s="2">
+        <v>2700</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="H49" t="s">
-        <v>132</v>
+        <v>94</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="I49" t="s">
-        <v>181</v>
-      </c>
-      <c r="J49">
-        <v>79.7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="J49" t="s">
+        <v>96</v>
+      </c>
+      <c r="K49">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="8">
+        <v>49</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="1">
+        <v>2</v>
+      </c>
+      <c r="E50" s="1">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="F50" s="2">
+        <v>6400</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I50" t="s">
+        <v>64</v>
+      </c>
+      <c r="J50" t="s">
+        <v>204</v>
+      </c>
+      <c r="K50">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="8">
         <v>50</v>
       </c>
-      <c r="C50" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="D50" s="1">
-        <v>-1.3</v>
-      </c>
-      <c r="E50" s="2">
-        <v>4750</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="H50" t="s">
-        <v>132</v>
-      </c>
-      <c r="I50" t="s">
-        <v>133</v>
-      </c>
-      <c r="J50">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>47</v>
-      </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D51" s="5">
+        <v>15.6</v>
+      </c>
+      <c r="E51" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="F51" s="6">
+        <v>9000</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="K51" s="4">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="8">
         <v>51</v>
       </c>
-      <c r="C51" s="1">
-        <v>2</v>
-      </c>
-      <c r="D51" s="1">
-        <v>-4.0999999999999996</v>
-      </c>
-      <c r="E51" s="2">
-        <v>6400</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H51" t="s">
-        <v>64</v>
-      </c>
-      <c r="I51" t="s">
-        <v>204</v>
-      </c>
-      <c r="J51">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>47</v>
-      </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D52" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="E52" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="F52" s="2">
+        <v>2600</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I52" t="s">
+        <v>79</v>
+      </c>
+      <c r="J52" t="s">
+        <v>90</v>
+      </c>
+      <c r="K52">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" s="8">
         <v>52</v>
       </c>
-      <c r="C52" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="D52" s="1">
-        <v>-9.5</v>
-      </c>
-      <c r="E52" s="2">
-        <v>5200</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H52" t="s">
-        <v>65</v>
-      </c>
-      <c r="I52" t="s">
-        <v>186</v>
-      </c>
-      <c r="J52">
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>47</v>
-      </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1</v>
+      </c>
+      <c r="E53" s="1">
+        <v>-3.6</v>
+      </c>
+      <c r="F53" s="2">
+        <v>19500</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="I53" t="s">
+        <v>79</v>
+      </c>
+      <c r="J53" t="s">
+        <v>176</v>
+      </c>
+      <c r="K53">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" s="8">
         <v>53</v>
       </c>
-      <c r="C53" s="1">
-        <v>14.1</v>
-      </c>
-      <c r="D53" s="1">
-        <v>12.3</v>
-      </c>
-      <c r="E53" s="2">
-        <v>10300</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H53" t="s">
-        <v>68</v>
-      </c>
-      <c r="I53" t="s">
-        <v>187</v>
-      </c>
-      <c r="J53">
-        <v>250</v>
+      <c r="C54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="E54" s="1">
+        <v>10.3</v>
+      </c>
+      <c r="F54" s="2">
+        <v>2950</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="8">
+        <v>54</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="E55" s="1">
+        <v>13.2</v>
+      </c>
+      <c r="F55" s="2">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" s="8">
+        <v>55</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D56" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="E56" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="F56" s="2">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" s="8">
+        <v>56</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" s="1">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E57" s="1">
+        <v>11.9</v>
+      </c>
+      <c r="F57" s="2">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>46</v>
+      </c>
+      <c r="B58" s="8">
+        <v>57</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1">
+        <v>-26.8</v>
+      </c>
+      <c r="E58" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="F58" s="2">
+        <v>5770</v>
+      </c>
+      <c r="J58" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E47">
-    <sortCondition ref="A2:A47"/>
+  <sortState ref="A2:K58">
+    <sortCondition ref="I2:I58"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>